<commit_message>
street name + city seperation algorithm updated but still not working 100% of the time as streets can have a subset of a city name
</commit_message>
<xml_diff>
--- a/Address List testing.xlsx
+++ b/Address List testing.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">4059 FARNSWORTH CRES   MISSISSAUGA ON,         L5L3Z4    </t>
+    <t>123 MARKHAM STREET NAME EXTRA WORDS ON A1A1A1</t>
   </si>
 </sst>
 </file>
@@ -346,9 +346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
adding street number calculations into street and city name algorithm
changing computers
</commit_message>
<xml_diff>
--- a/Address List testing.xlsx
+++ b/Address List testing.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesper\Documents\GitHub\opta-tech-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE67BB18-9EDE-49B8-BEA6-3CB231646769}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>123 MARKHAM STREET NAME EXTRA WORDS ON A1A1A1</t>
+    <t>562 WILLIAM BERCZY BLVD MARKHAM ON L6C2P7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -343,17 +344,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
street name + city name + street number algorithm still WIP
</commit_message>
<xml_diff>
--- a/Address List testing.xlsx
+++ b/Address List testing.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesper\Documents\GitHub\opta-tech-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE67BB18-9EDE-49B8-BEA6-3CB231646769}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,13 +26,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>562 WILLIAM BERCZY BLVD MARKHAM ON L6C2P7</t>
+    <t xml:space="preserve">6927    EDMONTON, AB         T5Z3S2    164 AVE  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -344,17 +343,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added a new case to street + city name algorithm, if street suffix is 2nd, 1st must be street name
</commit_message>
<xml_diff>
--- a/Address List testing.xlsx
+++ b/Address List testing.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">6927    EDMONTON, AB         T5Z3S2    164 AVE  </t>
+    <t>164 AVE EDMONTON AB T5Z3S2 6927</t>
   </si>
 </sst>
 </file>
@@ -347,7 +347,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
address parsing working printing to console in table format working writing to database WIP
</commit_message>
<xml_diff>
--- a/Address List testing.xlsx
+++ b/Address List testing.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>164 AVE EDMONTON AB T5Z3S2 6927</t>
+    <t xml:space="preserve">1605 BEACH RD.   N  SALT SPRING ISLAND,CAPITAL BC         V8K1A8    </t>
   </si>
 </sst>
 </file>
@@ -347,7 +347,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added N E S W to suffixes file to catch street names that end in a direction street suffix at the end case WIP TODO street suffix in the middle case
</commit_message>
<xml_diff>
--- a/Address List testing.xlsx
+++ b/Address List testing.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>164 AVE EDMONTON AB T5Z3S2 6927</t>
+    <t>6927 EDMONTON AB T5Z3S2 164 AVE</t>
   </si>
 </sst>
 </file>
@@ -347,7 +347,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
more cases for street name and city name parsing street ending in the middle cases WIP changing computer
</commit_message>
<xml_diff>
--- a/Address List testing.xlsx
+++ b/Address List testing.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesper\Documents\GitHub\opta-tech-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E2DE04-CF11-494E-9006-5379FF6310B1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>6927 EDMONTON AB T5Z3S2 164 AVE</t>
+    <t>BRIDLEFIELD LANE MARKHAM ON L6C2P3 61</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -343,19 +344,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
changed Lists to HashSets for storing province, city, suffixes
street name and city name parsing done !

TODO:
writing to SQL server
tabulated view in console
</commit_message>
<xml_diff>
--- a/Address List testing.xlsx
+++ b/Address List testing.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesper\Documents\GitHub\opta-tech-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E2DE04-CF11-494E-9006-5379FF6310B1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +24,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>BRIDLEFIELD LANE MARKHAM ON L6C2P3 61</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>562 WILLIAM BERCZY BLVD MARKHAM ON L6C2P7</t>
+  </si>
+  <si>
+    <t>MARKHAM WILLIAM BERCZY BLVD ON L6C2P7 562</t>
+  </si>
+  <si>
+    <t>WILLIAM BERCZY BLVD 562 ON L6C2P7 MARKHAM</t>
+  </si>
+  <si>
+    <t>WILLIAM BERCZY BLVD MARKHAM ON L6C2P7 562</t>
+  </si>
+  <si>
+    <t>562 MARKHAM ON L6C2P7 WILLIAM BERCZY BLVD</t>
+  </si>
+  <si>
+    <t>MARKHAM 562 ON L6C2P7 WILLIAM BERCZY BLVD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -344,19 +358,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed LoadXLS method name typo
</commit_message>
<xml_diff>
--- a/Address List testing.xlsx
+++ b/Address List testing.xlsx
@@ -24,9 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve">1605 BEACH RD.   N  SALT SPRING ISLAND,CAPITAL BC         V8K1A8    </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>562 WILLIAM BERCZY BLVD MARKHAM ON L6C2P7</t>
+  </si>
+  <si>
+    <t>MARKHAM WILLIAM BERCZY BLVD ON L6C2P7 562</t>
+  </si>
+  <si>
+    <t>WILLIAM BERCZY BLVD 562 ON L6C2P7 MARKHAM</t>
+  </si>
+  <si>
+    <t>WILLIAM BERCZY BLVD MARKHAM ON L6C2P7 562</t>
+  </si>
+  <si>
+    <t>562 MARKHAM ON L6C2P7 WILLIAM BERCZY BLVD</t>
+  </si>
+  <si>
+    <t>MARKHAM 562 ON L6C2P7 WILLIAM BERCZY BLVD</t>
   </si>
 </sst>
 </file>
@@ -344,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -360,6 +375,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
parsing algorithm working as intended
database operations all working
</commit_message>
<xml_diff>
--- a/Address List testing.xlsx
+++ b/Address List testing.xlsx
@@ -24,24 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>562 WILLIAM BERCZY BLVD MARKHAM ON L6C2P7</t>
-  </si>
-  <si>
-    <t>MARKHAM WILLIAM BERCZY BLVD ON L6C2P7 562</t>
-  </si>
-  <si>
-    <t>WILLIAM BERCZY BLVD 562 ON L6C2P7 MARKHAM</t>
-  </si>
-  <si>
-    <t>WILLIAM BERCZY BLVD MARKHAM ON L6C2P7 562</t>
-  </si>
-  <si>
-    <t>562 MARKHAM ON L6C2P7 WILLIAM BERCZY BLVD</t>
-  </si>
-  <si>
-    <t>MARKHAM 562 ON L6C2P7 WILLIAM BERCZY BLVD</t>
+    <t xml:space="preserve">107 OLD COLONY RD    RICHMOND HILL ON,         L4E3X2    </t>
   </si>
 </sst>
 </file>
@@ -359,11 +344,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -375,31 +358,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>